<commit_message>
save Hw Db xlsx file
</commit_message>
<xml_diff>
--- a/Seminars/HomeWork/Database/Seminar_2/HwDbTask.xlsx
+++ b/Seminars/HomeWork/Database/Seminar_2/HwDbTask.xlsx
@@ -482,13 +482,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -586,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -603,152 +609,164 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1061,516 +1079,516 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="29" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="55" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="57" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="58" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="59" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="14.4">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="32"/>
-      <c r="D1" s="34"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="43"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="32"/>
       <c r="B2" s="33"/>
       <c r="C2" s="32"/>
-      <c r="D2" s="34"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="32"/>
       <c r="B3" s="33"/>
       <c r="C3" s="32"/>
-      <c r="D3" s="34"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="43"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="32"/>
       <c r="B4" s="33"/>
       <c r="C4" s="32"/>
-      <c r="D4" s="34"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="43"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="32"/>
       <c r="B5" s="33"/>
       <c r="C5" s="32"/>
-      <c r="D5" s="34"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="43"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="32"/>
       <c r="B6" s="33"/>
       <c r="C6" s="32"/>
-      <c r="D6" s="34"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="8"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="7"/>
       <c r="E7" s="43"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="8"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="7"/>
       <c r="E8" s="43"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="7"/>
       <c r="E9" s="43"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="7"/>
       <c r="E10" s="43"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A11" s="46" t="s">
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A11" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="47" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A12" s="49" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A12" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="51">
         <v>32916</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="52">
         <v>126</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="50" t="s">
         <v>49</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A13" s="49" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B13" s="51">
         <v>32916</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="52">
         <v>127</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="50" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A14" s="49" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A14" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="50">
+      <c r="B14" s="51">
         <v>37152</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="52">
         <v>527</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="50" t="s">
         <v>50</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A15" s="49" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A15" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="50">
+      <c r="B15" s="51">
         <v>30429</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="52">
         <v>234</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="50" t="s">
         <v>51</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="50">
+      <c r="B16" s="51">
         <v>30430</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="52">
         <v>235</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="50" t="s">
         <v>51</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="50">
+      <c r="B17" s="51">
         <v>35936</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="52">
         <v>456</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="50" t="s">
         <v>52</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="50">
+      <c r="B18" s="51">
         <v>39276</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="52">
         <v>643</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="50" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="51">
         <v>39276</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="52">
         <v>654</v>
       </c>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="50" t="s">
         <v>51</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="51">
         <v>31841</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="52">
         <v>412</v>
       </c>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="50" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="51">
         <v>32736</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="52">
         <v>723</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="50" t="s">
         <v>49</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="50">
+      <c r="B22" s="51">
         <v>35438</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="52">
         <v>876</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="E22" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="50" t="s">
         <v>57</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="50">
+      <c r="B23" s="51">
         <v>35438</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="51">
+      <c r="D23" s="52">
         <v>875</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="49" t="s">
+      <c r="G23" s="50" t="s">
         <v>57</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="50">
+      <c r="B24" s="51">
         <v>35402</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="51">
+      <c r="D24" s="52">
         <v>933</v>
       </c>
-      <c r="E24" s="50" t="s">
+      <c r="E24" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="50" t="s">
         <v>49</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="8"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="7"/>
       <c r="E25" s="43"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="8"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="37"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="6"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="47" t="s">
+      <c r="E27" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="47" t="s">
         <v>7</v>
       </c>
       <c r="G27" s="6"/>
@@ -1578,20 +1596,20 @@
       <c r="I27" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="47" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="49" t="s">
+      <c r="F28" s="50" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="6"/>
@@ -1599,20 +1617,20 @@
       <c r="I28" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="50">
+      <c r="B29" s="51">
         <v>32916</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="49" t="s">
+      <c r="F29" s="50" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="6"/>
@@ -1620,70 +1638,70 @@
       <c r="I29" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="50">
+      <c r="B30" s="51">
         <v>32916</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="10"/>
-      <c r="E30" s="54"/>
+      <c r="E30" s="55"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="50">
+      <c r="B31" s="51">
         <v>37152</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="50" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="10"/>
-      <c r="E31" s="54"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="50">
+      <c r="B32" s="51">
         <v>30429</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="50" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="50">
+      <c r="B33" s="51">
         <v>30430</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="50" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="10"/>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="48" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="6"/>
@@ -1692,17 +1710,17 @@
       <c r="I33" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="50">
+      <c r="B34" s="51">
         <v>35936</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="50" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="10"/>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="51" t="s">
         <v>55</v>
       </c>
       <c r="F34" s="6"/>
@@ -1711,70 +1729,70 @@
       <c r="I34" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="50">
+      <c r="B35" s="51">
         <v>39276</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="50" t="s">
         <v>27</v>
       </c>
       <c r="D35" s="10"/>
-      <c r="E35" s="54"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="50">
+      <c r="B36" s="51">
         <v>39276</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="50" t="s">
         <v>27</v>
       </c>
       <c r="D36" s="10"/>
-      <c r="E36" s="54"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="50">
+      <c r="B37" s="51">
         <v>31841</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="50" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="8"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="44"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="50">
+      <c r="B38" s="51">
         <v>32736</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="50" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="10"/>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F38" s="6"/>
@@ -1783,17 +1801,17 @@
       <c r="I38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="50">
+      <c r="B39" s="51">
         <v>35438</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="10"/>
-      <c r="E39" s="50">
+      <c r="E39" s="51">
         <v>32916</v>
       </c>
       <c r="F39" s="6"/>
@@ -1802,17 +1820,17 @@
       <c r="I39" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="50">
+      <c r="B40" s="51">
         <v>35438</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D40" s="10"/>
-      <c r="E40" s="50">
+      <c r="E40" s="51">
         <v>32916</v>
       </c>
       <c r="F40" s="6"/>
@@ -1821,17 +1839,17 @@
       <c r="I40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="50">
+      <c r="B41" s="51">
         <v>35402</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="50" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="10"/>
-      <c r="E41" s="50">
+      <c r="E41" s="51">
         <v>30429</v>
       </c>
       <c r="F41" s="6"/>
@@ -1841,10 +1859,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A42" s="6"/>
-      <c r="B42" s="37"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="6"/>
       <c r="D42" s="10"/>
-      <c r="E42" s="50">
+      <c r="E42" s="51">
         <v>30430</v>
       </c>
       <c r="F42" s="6"/>
@@ -1854,10 +1872,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A43" s="6"/>
-      <c r="B43" s="37"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="10"/>
-      <c r="E43" s="50">
+      <c r="E43" s="51">
         <v>35402</v>
       </c>
       <c r="F43" s="6"/>
@@ -1888,15 +1906,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="41" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="40" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="29" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="41" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="41" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="41" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="30" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="30" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="30" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="30" width="14.147857142857141" customWidth="1" bestFit="1"/>
@@ -1913,13 +1931,13 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="8"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="10"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="34"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="32"/>
       <c r="C2" s="33"/>
       <c r="D2" s="32"/>
@@ -1927,13 +1945,13 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="8"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="10"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="34"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
       <c r="D3" s="32"/>
@@ -1941,13 +1959,13 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="10"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="32"/>
       <c r="C4" s="33"/>
       <c r="D4" s="32"/>
@@ -1955,13 +1973,13 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
+      <c r="I4" s="34"/>
       <c r="J4" s="10"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="32"/>
       <c r="C5" s="33"/>
       <c r="D5" s="32"/>
@@ -1969,13 +1987,13 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="10"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="35"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="8"/>
@@ -1983,13 +2001,13 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="10"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="35"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="8"/>
@@ -1997,7 +2015,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="10"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -2227,9 +2245,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A15" s="36"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="37"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="6"/>
       <c r="E15" s="10"/>
       <c r="F15" s="20">
@@ -2253,9 +2271,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A16" s="36"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="37"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="6"/>
       <c r="E16" s="10"/>
       <c r="F16" s="20">
@@ -2279,9 +2297,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A17" s="36"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="37"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="6"/>
       <c r="E17" s="10"/>
       <c r="F17" s="20">
@@ -2305,9 +2323,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A18" s="36"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="37"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="6"/>
       <c r="E18" s="10"/>
       <c r="F18" s="20">
@@ -2331,9 +2349,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A19" s="36"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="37"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="6"/>
       <c r="E19" s="10"/>
       <c r="F19" s="20">
@@ -2357,9 +2375,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A20" s="36"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="37"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="6"/>
       <c r="E20" s="10"/>
       <c r="F20" s="20">
@@ -2383,9 +2401,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A21" s="36"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="6"/>
       <c r="E21" s="10"/>
       <c r="F21" s="20">
@@ -2409,9 +2427,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A22" s="36"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="37"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="6"/>
       <c r="E22" s="10"/>
       <c r="F22" s="20">
@@ -2429,9 +2447,9 @@
       <c r="L22" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A23" s="36"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="37"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="6"/>
       <c r="E23" s="10"/>
       <c r="F23" s="20">
@@ -2449,7 +2467,7 @@
       <c r="L23" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="35"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="8"/>
@@ -2457,13 +2475,13 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="8"/>
+      <c r="I24" s="34"/>
       <c r="J24" s="10"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="35"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
@@ -2471,13 +2489,13 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="8"/>
+      <c r="I25" s="34"/>
       <c r="J25" s="10"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="35"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
@@ -2485,23 +2503,23 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="34"/>
       <c r="J26" s="10"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="8"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="8"/>
+      <c r="I27" s="34"/>
       <c r="J27" s="10"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -2693,7 +2711,7 @@
       <c r="L34" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="35"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="8"/>
@@ -2701,13 +2719,13 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="8"/>
+      <c r="I35" s="34"/>
       <c r="J35" s="10"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="35"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
       <c r="D36" s="8"/>
@@ -2715,23 +2733,23 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="8"/>
+      <c r="I36" s="34"/>
       <c r="J36" s="10"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="8"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="8"/>
+      <c r="I37" s="34"/>
       <c r="J37" s="10"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
@@ -2979,7 +2997,7 @@
       <c r="L46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="35"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="8"/>
@@ -2987,13 +3005,13 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="8"/>
+      <c r="I47" s="34"/>
       <c r="J47" s="10"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="35"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
       <c r="D48" s="8"/>
@@ -3001,23 +3019,23 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="8"/>
+      <c r="I48" s="34"/>
       <c r="J48" s="10"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="8"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="8"/>
+      <c r="I49" s="34"/>
       <c r="J49" s="10"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
@@ -3405,7 +3423,7 @@
       <c r="L63" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
-      <c r="A64" s="35"/>
+      <c r="A64" s="7"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
       <c r="D64" s="8"/>
@@ -3413,13 +3431,13 @@
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="6"/>
-      <c r="I64" s="8"/>
+      <c r="I64" s="34"/>
       <c r="J64" s="10"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
-      <c r="A65" s="35"/>
+      <c r="A65" s="7"/>
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="8"/>
@@ -3427,13 +3445,13 @@
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="6"/>
-      <c r="I65" s="8"/>
+      <c r="I65" s="34"/>
       <c r="J65" s="10"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
-      <c r="A66" s="35"/>
+      <c r="A66" s="7"/>
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
       <c r="D66" s="8"/>
@@ -3441,23 +3459,23 @@
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="6"/>
-      <c r="I66" s="8"/>
+      <c r="I66" s="34"/>
       <c r="J66" s="10"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
-      <c r="A67" s="38" t="s">
+      <c r="A67" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="39"/>
-      <c r="C67" s="40"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="39"/>
       <c r="D67" s="8"/>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
       <c r="H67" s="6"/>
-      <c r="I67" s="8"/>
+      <c r="I67" s="34"/>
       <c r="J67" s="10"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>

</xml_diff>

<commit_message>
added changes database HW sem 3
</commit_message>
<xml_diff>
--- a/Seminars/HomeWork/Database/Seminar_2/HwDbTask.xlsx
+++ b/Seminars/HomeWork/Database/Seminar_2/HwDbTask.xlsx
@@ -592,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,123 +609,123 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -756,17 +756,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1079,15 +1070,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="57" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="58" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="59" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="29" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="40" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="56" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="28" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1329,7 +1320,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A16" s="50" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1345,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A17" s="50" t="s">
         <v>22</v>
       </c>
@@ -1379,7 +1370,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A18" s="50" t="s">
         <v>53</v>
       </c>
@@ -1404,7 +1395,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A19" s="50" t="s">
         <v>53</v>
       </c>

</xml_diff>